<commit_message>
All the files used till this date
</commit_message>
<xml_diff>
--- a/detailed competitor for selection.xlsx
+++ b/detailed competitor for selection.xlsx
@@ -13,7 +13,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="aJUWlZssIEirvPVYVTvJ9/CjtGyFqmzFK74weSgpDys="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="4Zr00sBBgRoKrta5CNxurlGoIIJx2X6JoNThugEihxw="/>
     </ext>
   </extLst>
 </workbook>
@@ -25,6 +25,30 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="P20">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABhrd3hQs
+Aditya Gupta    (2025-04-11 23:45:41)
+Page 1 of form 990 and page 4 and 5 of audit report</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="O20">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABhrd3hQo
+Aditya Gupta    (2025-04-11 23:44:20)
+Audit page 4 "Management and general expenses" Page 5 "events and related expenses"</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="N20">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABhrd3hQk
+Aditya Gupta    (2025-04-11 23:40:57)
+form 990 page 2, audit report page 5 "grants and educational program"</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="S20">
       <text>
         <t xml:space="preserve">======
@@ -69,7 +93,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgRj66JrSEmgulHj5JxViNptS8W0A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mh8fiNXP+NPQEbU8bpmZU1YfBALpw=="/>
     </ext>
   </extLst>
 </comments>
@@ -108,7 +132,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mg1Q9NUSeeJJ0wHhqaTuaOgdMpQFg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgkQC6cWivoqg/XFNfXjvnpqlpoYQ=="/>
     </ext>
   </extLst>
 </comments>
@@ -131,14 +155,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miv2RjNtCqH2qshASELQy8wKYRglw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhZycNg32Az8V7OT6a+LcZCPflDxA=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="431">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -958,7 +982,7 @@
     <t>Contributions $117.67M
 Program service $2.77M
 Investment income $0.95M
-Total Revenue: $121.4M</t>
+Total Revenue: $121.3M</t>
   </si>
   <si>
     <t>Contributions $104.6M
@@ -979,7 +1003,7 @@
     <t>Educational initiatives, fundraising events</t>
   </si>
   <si>
-    <t>$0 as per the form 990 and their official website.</t>
+    <t>$2.7M</t>
   </si>
   <si>
     <t>11-50 as per linkedin, 10 as per form 990</t>
@@ -2244,6 +2268,12 @@
     </r>
   </si>
   <si>
+    <t>Contributions $117.67M
+Program service $2.77M
+Investment income $0.95M
+Total Revenue: $121.4M</t>
+  </si>
+  <si>
     <t>Contributions and Grants $29.5M
 Total Revenue: $34.5M</t>
   </si>
@@ -2253,6 +2283,9 @@
   </si>
   <si>
     <t>Grantmaking, collaborative funding initiatives.</t>
+  </si>
+  <si>
+    <t>$0 as per the form 990 and their official website.</t>
   </si>
   <si>
     <t>20+</t>
@@ -2876,7 +2909,7 @@
     <col customWidth="1" min="13" max="13" width="17.13"/>
     <col customWidth="1" min="14" max="14" width="23.13"/>
     <col customWidth="1" min="15" max="15" width="18.5"/>
-    <col customWidth="1" min="16" max="16" width="14.88"/>
+    <col customWidth="1" min="16" max="16" width="18.88"/>
     <col customWidth="1" min="17" max="17" width="29.38"/>
     <col customWidth="1" min="18" max="18" width="22.13"/>
     <col customWidth="1" min="19" max="20" width="34.88"/>
@@ -57548,10 +57581,10 @@
         <v>208</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>217</v>
+        <v>415</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="46"/>
@@ -57581,7 +57614,7 @@
         <v>218</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H6" s="46"/>
       <c r="I6" s="46"/>
@@ -57686,7 +57719,7 @@
         <v>212</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="G10" s="52" t="s">
         <v>235</v>
@@ -57730,7 +57763,7 @@
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>
       <c r="F12" s="52" t="s">
-        <v>223</v>
+        <v>419</v>
       </c>
       <c r="G12" s="56"/>
       <c r="H12" s="46"/>
@@ -57773,7 +57806,7 @@
         <v>78</v>
       </c>
       <c r="G14" s="52" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="H14" s="46"/>
       <c r="I14" s="46"/>
@@ -57888,22 +57921,22 @@
         <v>387</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="F20" s="52" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="G20" s="52" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="H20" s="46"/>
       <c r="I20" s="46"/>
@@ -57915,7 +57948,7 @@
     </row>
     <row r="21">
       <c r="A21" s="48" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B21" s="58" t="s">
         <v>180</v>
@@ -57945,17 +57978,17 @@
     </row>
     <row r="22">
       <c r="A22" s="48" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B22" s="56"/>
       <c r="C22" s="56"/>
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
       <c r="F22" s="52" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="G22" s="52" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="H22" s="46"/>
       <c r="I22" s="46"/>

</xml_diff>